<commit_message>
probably function generic stack move
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://streamrealty-my.sharepoint.com/personal/jgilles_streamdatacenters_com/Documents/Documents/GitHub/baker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDE9641D-C63C-48DB-BD3F-A440A3CA374E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="228" documentId="8_{FDE9641D-C63C-48DB-BD3F-A440A3CA374E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{352F7BDC-17AB-48F5-82C2-5BE2E95AE373}"/>
   <bookViews>
-    <workbookView xWindow="-22965" yWindow="2580" windowWidth="21600" windowHeight="11385" xr2:uid="{DFAEEB24-EB5D-4485-9BE1-8205848800AE}"/>
+    <workbookView xWindow="-28800" yWindow="135" windowWidth="11400" windowHeight="15600" xr2:uid="{DFAEEB24-EB5D-4485-9BE1-8205848800AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>pack</t>
   </si>
@@ -69,9 +69,6 @@
     <t>f</t>
   </si>
   <si>
-    <t>Open spaces</t>
-  </si>
-  <si>
     <t>Cards</t>
   </si>
   <si>
@@ -127,6 +124,27 @@
   </si>
   <si>
     <t>unpack spaces</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Open spaces (including destination)</t>
   </si>
 </sst>
 </file>
@@ -286,10 +304,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -300,13 +317,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -334,9 +349,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -374,7 +389,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -480,7 +495,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -622,7 +637,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -632,49 +647,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5254F136-A2AE-4FA7-9115-E6273F9CD59D}">
   <dimension ref="A2:Y47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="11">
+      <c r="W2" s="8"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
       </c>
       <c r="H3" t="s">
         <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>3</v>
-      </c>
-      <c r="W3" s="12">
-        <v>1</v>
-      </c>
-      <c r="X3" s="13">
+        <v>28</v>
+      </c>
+      <c r="W3" s="11">
+        <v>1</v>
+      </c>
+      <c r="X3">
         <f>2^(W3-1)</f>
         <v>1</v>
       </c>
-      <c r="Y3" s="3">
-        <f>X3*$Y$2</f>
+      <c r="Y3" s="2">
+        <f t="shared" ref="Y3:Y8" si="0">X3*$Y$2</f>
         <v>2</v>
       </c>
     </row>
@@ -698,37 +712,37 @@
       <c r="H4">
         <v>16</v>
       </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="6">
-        <v>1</v>
-      </c>
-      <c r="N4" s="6">
+      <c r="L4" s="4"/>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
+        <v>1</v>
+      </c>
+      <c r="O4" s="5">
         <v>2</v>
       </c>
-      <c r="O4" s="6">
+      <c r="P4" s="5">
         <v>3</v>
       </c>
-      <c r="P4" s="6">
-        <v>4</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>5</v>
-      </c>
-      <c r="R4" s="6">
+      <c r="Q4" s="5">
+        <v>4</v>
+      </c>
+      <c r="R4" s="5">
+        <v>5</v>
+      </c>
+      <c r="S4" s="5">
         <v>6</v>
       </c>
-      <c r="S4" s="6">
-        <v>7</v>
-      </c>
-      <c r="W4" s="12">
+      <c r="W4" s="11">
         <v>2</v>
       </c>
-      <c r="X4" s="13">
-        <f t="shared" ref="X4:X8" si="0">2^(W4-1)</f>
+      <c r="X4">
+        <f t="shared" ref="X4:X8" si="1">2^(W4-1)</f>
         <v>2</v>
       </c>
-      <c r="Y4" s="3">
-        <f>X4*$Y$2</f>
+      <c r="Y4" s="2">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -746,41 +760,41 @@
         <v>15</v>
       </c>
       <c r="K5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" s="4">
-        <v>1</v>
-      </c>
-      <c r="M5" s="7">
-        <v>1</v>
-      </c>
-      <c r="N5" s="8">
-        <v>1</v>
-      </c>
-      <c r="O5" s="8">
-        <v>1</v>
-      </c>
-      <c r="P5" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="8">
-        <v>1</v>
-      </c>
-      <c r="R5" s="8">
-        <v>1</v>
-      </c>
-      <c r="S5" s="8">
-        <v>1</v>
-      </c>
-      <c r="W5" s="12">
         <v>3</v>
       </c>
-      <c r="X5" s="13">
+      <c r="L5" s="3">
+        <v>1</v>
+      </c>
+      <c r="M5" s="6">
+        <v>1</v>
+      </c>
+      <c r="N5" s="7">
+        <v>1</v>
+      </c>
+      <c r="O5" s="7">
+        <v>1</v>
+      </c>
+      <c r="P5" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>1</v>
+      </c>
+      <c r="R5" s="7">
+        <v>1</v>
+      </c>
+      <c r="S5" s="7">
+        <v>1</v>
+      </c>
+      <c r="W5" s="11">
+        <v>3</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Y5" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="Y5" s="3">
-        <f>X5*$Y$2</f>
         <v>8</v>
       </c>
     </row>
@@ -797,39 +811,39 @@
       <c r="H6">
         <v>14</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="3">
         <v>2</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N6" s="6">
         <v>3</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="7">
         <v>3</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="7">
         <v>3</v>
       </c>
-      <c r="Q6" s="8">
+      <c r="Q6" s="7">
         <v>3</v>
       </c>
-      <c r="R6" s="8">
+      <c r="R6" s="7">
         <v>3</v>
       </c>
-      <c r="S6" s="8">
+      <c r="S6" s="7">
         <v>3</v>
       </c>
-      <c r="W6" s="12">
-        <v>4</v>
-      </c>
-      <c r="X6" s="13">
+      <c r="W6" s="11">
+        <v>4</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Y6" s="2">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="Y6" s="3">
-        <f>X6*$Y$2</f>
         <v>16</v>
       </c>
     </row>
@@ -840,7 +854,7 @@
       <c r="H7">
         <v>13</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="3">
         <v>3</v>
       </c>
       <c r="M7">
@@ -849,30 +863,30 @@
       <c r="N7">
         <v>0</v>
       </c>
-      <c r="O7" s="16">
-        <v>5</v>
-      </c>
-      <c r="P7" s="16">
-        <v>5</v>
-      </c>
-      <c r="Q7" s="8">
-        <v>5</v>
-      </c>
-      <c r="R7" s="8">
-        <v>5</v>
-      </c>
-      <c r="S7" s="8">
-        <v>5</v>
-      </c>
-      <c r="W7" s="12">
-        <v>5</v>
-      </c>
-      <c r="X7" s="13">
+      <c r="O7" s="14">
+        <v>5</v>
+      </c>
+      <c r="P7" s="14">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>5</v>
+      </c>
+      <c r="R7" s="7">
+        <v>5</v>
+      </c>
+      <c r="S7" s="7">
+        <v>5</v>
+      </c>
+      <c r="W7" s="11">
+        <v>5</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="Y7" s="2">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="Y7" s="3">
-        <f>X7*$Y$2</f>
         <v>32</v>
       </c>
     </row>
@@ -880,7 +894,7 @@
       <c r="H8">
         <v>12</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="3">
         <v>4</v>
       </c>
       <c r="M8">
@@ -889,30 +903,30 @@
       <c r="N8">
         <v>0</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O8" s="15">
         <v>9</v>
       </c>
-      <c r="P8" s="16">
+      <c r="P8" s="14">
         <v>7</v>
       </c>
-      <c r="Q8" s="8">
+      <c r="Q8" s="7">
         <v>7</v>
       </c>
-      <c r="R8" s="8">
+      <c r="R8" s="7">
         <v>7</v>
       </c>
-      <c r="S8" s="8">
+      <c r="S8" s="7">
         <v>7</v>
       </c>
-      <c r="W8" s="14">
+      <c r="W8" s="12">
         <v>6</v>
       </c>
-      <c r="X8" s="15">
+      <c r="X8" s="13">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="Y8" s="4">
         <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="Y8" s="5">
-        <f>X8*$Y$2</f>
         <v>64</v>
       </c>
     </row>
@@ -920,7 +934,7 @@
       <c r="H9">
         <v>11</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="3">
         <v>5</v>
       </c>
       <c r="M9">
@@ -935,13 +949,13 @@
       <c r="P9">
         <v>11</v>
       </c>
-      <c r="Q9" s="8">
+      <c r="Q9" s="7">
         <v>9</v>
       </c>
-      <c r="R9" s="8">
+      <c r="R9" s="7">
         <v>9</v>
       </c>
-      <c r="S9" s="8">
+      <c r="S9" s="7">
         <v>9</v>
       </c>
     </row>
@@ -949,7 +963,7 @@
       <c r="H10">
         <v>10</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="3">
         <v>6</v>
       </c>
       <c r="M10">
@@ -961,16 +975,16 @@
       <c r="O10">
         <v>0</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10">
         <v>15</v>
       </c>
-      <c r="Q10" s="8">
+      <c r="Q10" s="7">
         <v>13</v>
       </c>
-      <c r="R10" s="8">
+      <c r="R10" s="7">
         <v>11</v>
       </c>
-      <c r="S10" s="8">
+      <c r="S10" s="7">
         <v>11</v>
       </c>
     </row>
@@ -978,7 +992,7 @@
       <c r="H11">
         <v>9</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="3">
         <v>7</v>
       </c>
       <c r="M11">
@@ -990,25 +1004,21 @@
       <c r="O11">
         <v>0</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11">
         <v>19</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="Q11">
         <v>17</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R11">
         <v>15</v>
       </c>
-      <c r="S11" s="8">
+      <c r="S11" s="7">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="L12" s="4">
+      <c r="L12" s="3">
         <v>8</v>
       </c>
       <c r="M12">
@@ -1020,30 +1030,30 @@
       <c r="O12">
         <v>0</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12" s="6">
         <v>25</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="Q12">
         <v>21</v>
       </c>
-      <c r="R12" s="2">
+      <c r="R12">
         <v>19</v>
       </c>
-      <c r="S12" s="2">
+      <c r="S12">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
       <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="L13" s="4">
+        <v>18</v>
+      </c>
+      <c r="L13" s="3">
         <v>9</v>
       </c>
       <c r="M13">
@@ -1055,31 +1065,31 @@
       <c r="O13">
         <v>0</v>
       </c>
-      <c r="P13" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="2">
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
         <v>25</v>
       </c>
-      <c r="R13" s="2">
+      <c r="R13">
         <v>23</v>
       </c>
-      <c r="S13" s="2">
+      <c r="S13">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
+      <c r="A14" s="16">
         <v>16</v>
       </c>
-      <c r="B14" s="18">
-        <v>6</v>
-      </c>
-      <c r="C14" s="8">
+      <c r="B14" s="16">
+        <v>5</v>
+      </c>
+      <c r="C14" s="7">
         <f>MIN(J17:J32)</f>
-        <v>51</v>
-      </c>
-      <c r="L14" s="4">
+        <v>71</v>
+      </c>
+      <c r="L14" s="3">
         <v>10</v>
       </c>
       <c r="M14">
@@ -1091,32 +1101,32 @@
       <c r="O14">
         <v>0</v>
       </c>
-      <c r="P14" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="19">
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
         <v>29</v>
       </c>
-      <c r="R14" s="2">
+      <c r="R14">
         <v>27</v>
       </c>
-      <c r="S14" s="2">
+      <c r="S14">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="2"/>
       <c r="G15" t="s">
-        <v>15</v>
-      </c>
-      <c r="L15" s="4">
+        <v>14</v>
+      </c>
+      <c r="L15" s="3">
         <v>11</v>
       </c>
       <c r="M15">
@@ -1128,53 +1138,53 @@
       <c r="O15">
         <v>0</v>
       </c>
-      <c r="P15" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="19">
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
         <v>33</v>
       </c>
-      <c r="R15" s="2">
+      <c r="R15">
         <v>31</v>
       </c>
-      <c r="S15" s="2">
+      <c r="S15">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
         <v>11</v>
       </c>
-      <c r="B16" t="s">
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="L16" s="3">
         <v>12</v>
       </c>
-      <c r="E16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" t="s">
-        <v>18</v>
-      </c>
-      <c r="L16" s="4">
-        <v>12</v>
-      </c>
       <c r="M16">
         <v>0</v>
       </c>
@@ -1184,16 +1194,16 @@
       <c r="O16">
         <v>0</v>
       </c>
-      <c r="P16" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="19">
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
         <v>39</v>
       </c>
-      <c r="R16" s="2">
+      <c r="R16">
         <v>35</v>
       </c>
-      <c r="S16" s="2">
+      <c r="S16">
         <v>33</v>
       </c>
     </row>
@@ -1202,32 +1212,32 @@
         <v>1</v>
       </c>
       <c r="B17">
-        <f>$B$14</f>
-        <v>6</v>
-      </c>
-      <c r="C17" s="3" cm="1">
+        <f t="shared" ref="B17:B32" si="2">$B$14</f>
+        <v>5</v>
+      </c>
+      <c r="C17" s="2" cm="1">
         <f t="array" ref="C17">IF(A17&gt;0,INDEX($M$5:$S$20,A17,B17),0)</f>
         <v>1</v>
       </c>
       <c r="D17">
-        <f>$A$14-A17</f>
+        <f t="shared" ref="D17:D32" si="3">$A$14-A17</f>
         <v>15</v>
       </c>
       <c r="E17">
-        <f>$B$14-1</f>
-        <v>5</v>
-      </c>
-      <c r="F17" s="3" cm="1">
+        <f t="shared" ref="E17:E32" si="4">$B$14-1</f>
+        <v>4</v>
+      </c>
+      <c r="F17" s="2" cm="1">
         <f t="array" ref="F17">IF(D17&gt;0,INDEX($M$5:$S$20,D17,E17),0)</f>
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <f>A17</f>
         <v>1</v>
       </c>
       <c r="H17">
-        <f>$B$14-1</f>
-        <v>5</v>
+        <f t="shared" ref="H17:H32" si="5">$B$14-1</f>
+        <v>4</v>
       </c>
       <c r="I17" cm="1">
         <f t="array" ref="I17">IF(G17&gt;0,INDEX($M$5:$S$20,G17,H17),0)</f>
@@ -1235,9 +1245,9 @@
       </c>
       <c r="J17">
         <f>IF(OR(C17=0,F17=0,I17=0),1000,C17+F17+I17)</f>
-        <v>63</v>
-      </c>
-      <c r="L17" s="4">
+        <v>1000</v>
+      </c>
+      <c r="L17" s="3">
         <v>13</v>
       </c>
       <c r="M17">
@@ -1249,16 +1259,16 @@
       <c r="O17">
         <v>0</v>
       </c>
-      <c r="P17" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="19">
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
         <v>45</v>
       </c>
-      <c r="R17" s="2">
+      <c r="R17">
         <v>39</v>
       </c>
-      <c r="S17" s="2">
+      <c r="S17">
         <v>37</v>
       </c>
     </row>
@@ -1267,42 +1277,42 @@
         <v>2</v>
       </c>
       <c r="B18">
-        <f>$B$14</f>
-        <v>6</v>
-      </c>
-      <c r="C18" s="3" cm="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" cm="1">
         <f t="array" ref="C18">IF(A18&gt;0,INDEX($M$5:$S$20,A18,B18),0)</f>
         <v>3</v>
       </c>
       <c r="D18">
-        <f>$A$14-A18</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="E18">
-        <f>$B$14-1</f>
-        <v>5</v>
-      </c>
-      <c r="F18" s="3" cm="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F18" s="2" cm="1">
         <f t="array" ref="F18">IF(D18&gt;0,INDEX($M$5:$S$20,D18,E18),0)</f>
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <f t="shared" ref="G18:G32" si="1">A18</f>
+        <f t="shared" ref="G18:G32" si="6">A18</f>
         <v>2</v>
       </c>
       <c r="H18">
-        <f>$B$14-1</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="I18" cm="1">
         <f t="array" ref="I18">IF(G18&gt;0,INDEX($M$5:$S$20,G18,H18),0)</f>
         <v>3</v>
       </c>
       <c r="J18">
-        <f t="shared" ref="J18:J32" si="2">IF(OR(C18=0,F18=0,I18=0),1000,C18+F18+I18)</f>
-        <v>59</v>
-      </c>
-      <c r="L18" s="4">
+        <f t="shared" ref="J18:J32" si="7">IF(OR(C18=0,F18=0,I18=0),1000,C18+F18+I18)</f>
+        <v>1000</v>
+      </c>
+      <c r="L18" s="3">
         <v>14</v>
       </c>
       <c r="M18">
@@ -1314,16 +1324,16 @@
       <c r="O18">
         <v>0</v>
       </c>
-      <c r="P18" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="19">
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
         <v>53</v>
       </c>
-      <c r="R18" s="2">
+      <c r="R18">
         <v>43</v>
       </c>
-      <c r="S18" s="2">
+      <c r="S18">
         <v>41</v>
       </c>
     </row>
@@ -1332,42 +1342,42 @@
         <v>3</v>
       </c>
       <c r="B19">
-        <f>$B$14</f>
-        <v>6</v>
-      </c>
-      <c r="C19" s="3" cm="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C19" s="2" cm="1">
         <f t="array" ref="C19">IF(A19&gt;0,INDEX($M$5:$S$20,A19,B19),0)</f>
         <v>5</v>
       </c>
       <c r="D19">
-        <f>$A$14-A19</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="E19">
-        <f>$B$14-1</f>
-        <v>5</v>
-      </c>
-      <c r="F19" s="3" cm="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F19" s="2" cm="1">
         <f t="array" ref="F19">IF(D19&gt;0,INDEX($M$5:$S$20,D19,E19),0)</f>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="H19">
-        <f>$B$14-1</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="I19" cm="1">
         <f t="array" ref="I19">IF(G19&gt;0,INDEX($M$5:$S$20,G19,H19),0)</f>
         <v>5</v>
       </c>
       <c r="J19">
-        <f t="shared" si="2"/>
-        <v>55</v>
-      </c>
-      <c r="L19" s="4">
+        <f t="shared" si="7"/>
+        <v>1000</v>
+      </c>
+      <c r="L19" s="3">
         <v>15</v>
       </c>
       <c r="M19">
@@ -1379,16 +1389,16 @@
       <c r="O19">
         <v>0</v>
       </c>
-      <c r="P19" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="19">
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
         <v>61</v>
       </c>
-      <c r="R19" s="2">
+      <c r="R19">
         <v>47</v>
       </c>
-      <c r="S19" s="2">
+      <c r="S19">
         <v>45</v>
       </c>
     </row>
@@ -1397,42 +1407,42 @@
         <v>4</v>
       </c>
       <c r="B20">
-        <f>$B$14</f>
-        <v>6</v>
-      </c>
-      <c r="C20" s="3" cm="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" cm="1">
         <f t="array" ref="C20">IF(A20&gt;0,INDEX($M$5:$S$20,A20,B20),0)</f>
         <v>7</v>
       </c>
       <c r="D20">
-        <f>$A$14-A20</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="E20">
-        <f>$B$14-1</f>
-        <v>5</v>
-      </c>
-      <c r="F20" s="3" cm="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F20" s="2" cm="1">
         <f t="array" ref="F20">IF(D20&gt;0,INDEX($M$5:$S$20,D20,E20),0)</f>
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="H20">
-        <f>$B$14-1</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="I20" cm="1">
         <f t="array" ref="I20">IF(G20&gt;0,INDEX($M$5:$S$20,G20,H20),0)</f>
         <v>7</v>
       </c>
       <c r="J20">
-        <f t="shared" si="2"/>
-        <v>53</v>
-      </c>
-      <c r="L20" s="4">
+        <f t="shared" si="7"/>
+        <v>1000</v>
+      </c>
+      <c r="L20" s="3">
         <v>16</v>
       </c>
       <c r="M20">
@@ -1444,16 +1454,16 @@
       <c r="O20">
         <v>0</v>
       </c>
-      <c r="P20" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="7">
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="6">
         <v>71</v>
       </c>
-      <c r="R20" s="2">
+      <c r="R20">
         <v>51</v>
       </c>
-      <c r="S20" s="2">
+      <c r="S20">
         <v>49</v>
       </c>
     </row>
@@ -1462,40 +1472,40 @@
         <v>5</v>
       </c>
       <c r="B21">
-        <f>$B$14</f>
-        <v>6</v>
-      </c>
-      <c r="C21" s="3" cm="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C21" s="2" cm="1">
         <f t="array" ref="C21">IF(A21&gt;0,INDEX($M$5:$S$20,A21,B21),0)</f>
         <v>9</v>
       </c>
       <c r="D21">
-        <f>$A$14-A21</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="E21">
-        <f>$B$14-1</f>
-        <v>5</v>
-      </c>
-      <c r="F21" s="3" cm="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F21" s="2" cm="1">
         <f t="array" ref="F21">IF(D21&gt;0,INDEX($M$5:$S$20,D21,E21),0)</f>
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="H21">
-        <f>$B$14-1</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="I21" cm="1">
         <f t="array" ref="I21">IF(G21&gt;0,INDEX($M$5:$S$20,G21,H21),0)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J21">
-        <f t="shared" si="2"/>
-        <v>51</v>
+        <f t="shared" si="7"/>
+        <v>1000</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -1503,40 +1513,40 @@
         <v>6</v>
       </c>
       <c r="B22">
-        <f>$B$14</f>
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" cm="1">
+        <f t="array" ref="C22">IF(A22&gt;0,INDEX($M$5:$S$20,A22,B22),0)</f>
+        <v>13</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F22" s="2" cm="1">
+        <f t="array" ref="F22">IF(D22&gt;0,INDEX($M$5:$S$20,D22,E22),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="C22" s="3" cm="1">
-        <f t="array" ref="C22">IF(A22&gt;0,INDEX($M$5:$S$20,A22,B22),0)</f>
-        <v>11</v>
-      </c>
-      <c r="D22">
-        <f>$A$14-A22</f>
-        <v>10</v>
-      </c>
-      <c r="E22">
-        <f>$B$14-1</f>
-        <v>5</v>
-      </c>
-      <c r="F22" s="3" cm="1">
-        <f t="array" ref="F22">IF(D22&gt;0,INDEX($M$5:$S$20,D22,E22),0)</f>
-        <v>29</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
       <c r="H22">
-        <f>$B$14-1</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="I22" cm="1">
         <f t="array" ref="I22">IF(G22&gt;0,INDEX($M$5:$S$20,G22,H22),0)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J22">
-        <f t="shared" si="2"/>
-        <v>53</v>
+        <f t="shared" si="7"/>
+        <v>1000</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -1544,40 +1554,40 @@
         <v>7</v>
       </c>
       <c r="B23">
-        <f>$B$14</f>
-        <v>6</v>
-      </c>
-      <c r="C23" s="3" cm="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C23" s="2" cm="1">
         <f t="array" ref="C23">IF(A23&gt;0,INDEX($M$5:$S$20,A23,B23),0)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D23">
-        <f>$A$14-A23</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="E23">
-        <f>$B$14-1</f>
-        <v>5</v>
-      </c>
-      <c r="F23" s="3" cm="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F23" s="2" cm="1">
         <f t="array" ref="F23">IF(D23&gt;0,INDEX($M$5:$S$20,D23,E23),0)</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="H23">
-        <f>$B$14-1</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="I23" cm="1">
         <f t="array" ref="I23">IF(G23&gt;0,INDEX($M$5:$S$20,G23,H23),0)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J23">
-        <f t="shared" si="2"/>
-        <v>57</v>
+        <f t="shared" si="7"/>
+        <v>1000</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -1585,40 +1595,40 @@
         <v>8</v>
       </c>
       <c r="B24">
-        <f>$B$14</f>
-        <v>6</v>
-      </c>
-      <c r="C24" s="3" cm="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C24" s="2" cm="1">
         <f t="array" ref="C24">IF(A24&gt;0,INDEX($M$5:$S$20,A24,B24),0)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D24">
-        <f>$A$14-A24</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="E24">
-        <f>$B$14-1</f>
-        <v>5</v>
-      </c>
-      <c r="F24" s="3" cm="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F24" s="2" cm="1">
         <f t="array" ref="F24">IF(D24&gt;0,INDEX($M$5:$S$20,D24,E24),0)</f>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="H24">
-        <f>$B$14-1</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="I24" cm="1">
         <f t="array" ref="I24">IF(G24&gt;0,INDEX($M$5:$S$20,G24,H24),0)</f>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J24">
-        <f t="shared" si="2"/>
-        <v>61</v>
+        <f t="shared" si="7"/>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -1626,40 +1636,58 @@
         <v>9</v>
       </c>
       <c r="B25">
-        <f>$B$14</f>
-        <v>6</v>
-      </c>
-      <c r="C25" s="3" cm="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C25" s="2" cm="1">
         <f t="array" ref="C25">IF(A25&gt;0,INDEX($M$5:$S$20,A25,B25),0)</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D25">
-        <f>$A$14-A25</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="E25">
-        <f>$B$14-1</f>
-        <v>5</v>
-      </c>
-      <c r="F25" s="3" cm="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F25" s="2" cm="1">
         <f t="array" ref="F25">IF(D25&gt;0,INDEX($M$5:$S$20,D25,E25),0)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="H25">
-        <f>$B$14-1</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="I25" cm="1">
         <f t="array" ref="I25">IF(G25&gt;0,INDEX($M$5:$S$20,G25,H25),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="7"/>
+        <v>1000</v>
+      </c>
+      <c r="M25" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O25" t="s">
+        <v>24</v>
+      </c>
+      <c r="P25" t="s">
         <v>25</v>
       </c>
-      <c r="J25">
-        <f t="shared" si="2"/>
-        <v>65</v>
+      <c r="Q25" t="s">
+        <v>26</v>
+      </c>
+      <c r="R25" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -1667,40 +1695,43 @@
         <v>10</v>
       </c>
       <c r="B26">
-        <f>$B$14</f>
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C26" s="2" cm="1">
+        <f t="array" ref="C26">IF(A26&gt;0,INDEX($M$5:$S$20,A26,B26),0)</f>
+        <v>29</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="C26" s="3" cm="1">
-        <f t="array" ref="C26">IF(A26&gt;0,INDEX($M$5:$S$20,A26,B26),0)</f>
-        <v>27</v>
-      </c>
-      <c r="D26">
-        <f>$A$14-A26</f>
-        <v>6</v>
-      </c>
       <c r="E26">
-        <f>$B$14-1</f>
-        <v>5</v>
-      </c>
-      <c r="F26" s="3" cm="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F26" s="2" cm="1">
         <f t="array" ref="F26">IF(D26&gt;0,INDEX($M$5:$S$20,D26,E26),0)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="H26">
-        <f>$B$14-1</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="I26" cm="1">
         <f t="array" ref="I26">IF(G26&gt;0,INDEX($M$5:$S$20,G26,H26),0)</f>
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <f t="shared" si="2"/>
-        <v>69</v>
+        <f t="shared" si="7"/>
+        <v>1000</v>
+      </c>
+      <c r="N26">
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -1708,40 +1739,43 @@
         <v>11</v>
       </c>
       <c r="B27">
-        <f>$B$14</f>
-        <v>6</v>
-      </c>
-      <c r="C27" s="3" cm="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C27" s="2" cm="1">
         <f t="array" ref="C27">IF(A27&gt;0,INDEX($M$5:$S$20,A27,B27),0)</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D27">
-        <f>$A$14-A27</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="E27">
-        <f>$B$14-1</f>
-        <v>5</v>
-      </c>
-      <c r="F27" s="3" cm="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F27" s="2" cm="1">
         <f t="array" ref="F27">IF(D27&gt;0,INDEX($M$5:$S$20,D27,E27),0)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="H27">
-        <f>$B$14-1</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="I27" cm="1">
         <f t="array" ref="I27">IF(G27&gt;0,INDEX($M$5:$S$20,G27,H27),0)</f>
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="J27">
-        <f t="shared" si="2"/>
-        <v>73</v>
+        <f t="shared" si="7"/>
+        <v>1000</v>
+      </c>
+      <c r="N27">
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -1749,40 +1783,43 @@
         <v>12</v>
       </c>
       <c r="B28">
-        <f>$B$14</f>
-        <v>6</v>
-      </c>
-      <c r="C28" s="3" cm="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C28" s="2" cm="1">
         <f t="array" ref="C28">IF(A28&gt;0,INDEX($M$5:$S$20,A28,B28),0)</f>
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D28">
-        <f>$A$14-A28</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E28">
-        <f>$B$14-1</f>
-        <v>5</v>
-      </c>
-      <c r="F28" s="3" cm="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F28" s="2" cm="1">
         <f t="array" ref="F28">IF(D28&gt;0,INDEX($M$5:$S$20,D28,E28),0)</f>
         <v>7</v>
       </c>
       <c r="G28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="H28">
-        <f>$B$14-1</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="I28" cm="1">
         <f t="array" ref="I28">IF(G28&gt;0,INDEX($M$5:$S$20,G28,H28),0)</f>
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <f t="shared" si="2"/>
-        <v>81</v>
+        <f t="shared" si="7"/>
+        <v>1000</v>
+      </c>
+      <c r="N28">
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -1790,40 +1827,43 @@
         <v>13</v>
       </c>
       <c r="B29">
-        <f>$B$14</f>
-        <v>6</v>
-      </c>
-      <c r="C29" s="3" cm="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C29" s="2" cm="1">
         <f t="array" ref="C29">IF(A29&gt;0,INDEX($M$5:$S$20,A29,B29),0)</f>
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D29">
-        <f>$A$14-A29</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E29">
-        <f>$B$14-1</f>
-        <v>5</v>
-      </c>
-      <c r="F29" s="3" cm="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F29" s="2" cm="1">
         <f t="array" ref="F29">IF(D29&gt;0,INDEX($M$5:$S$20,D29,E29),0)</f>
         <v>5</v>
       </c>
       <c r="G29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="H29">
-        <f>$B$14-1</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="I29" cm="1">
         <f t="array" ref="I29">IF(G29&gt;0,INDEX($M$5:$S$20,G29,H29),0)</f>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="J29">
-        <f t="shared" si="2"/>
-        <v>89</v>
+        <f t="shared" si="7"/>
+        <v>1000</v>
+      </c>
+      <c r="N29">
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -1831,40 +1871,43 @@
         <v>14</v>
       </c>
       <c r="B30">
-        <f>$B$14</f>
-        <v>6</v>
-      </c>
-      <c r="C30" s="3" cm="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C30" s="2" cm="1">
         <f t="array" ref="C30">IF(A30&gt;0,INDEX($M$5:$S$20,A30,B30),0)</f>
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D30">
-        <f>$A$14-A30</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E30">
-        <f>$B$14-1</f>
-        <v>5</v>
-      </c>
-      <c r="F30" s="3" cm="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F30" s="2" cm="1">
         <f t="array" ref="F30">IF(D30&gt;0,INDEX($M$5:$S$20,D30,E30),0)</f>
         <v>3</v>
       </c>
       <c r="G30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="H30">
-        <f>$B$14-1</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="I30" cm="1">
         <f t="array" ref="I30">IF(G30&gt;0,INDEX($M$5:$S$20,G30,H30),0)</f>
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="J30">
-        <f t="shared" si="2"/>
-        <v>99</v>
+        <f t="shared" si="7"/>
+        <v>1000</v>
+      </c>
+      <c r="N30">
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -1872,40 +1915,43 @@
         <v>15</v>
       </c>
       <c r="B31">
-        <f>$B$14</f>
-        <v>6</v>
-      </c>
-      <c r="C31" s="3" cm="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C31" s="2" cm="1">
         <f t="array" ref="C31">IF(A31&gt;0,INDEX($M$5:$S$20,A31,B31),0)</f>
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D31">
-        <f>$A$14-A31</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E31">
-        <f>$B$14-1</f>
-        <v>5</v>
-      </c>
-      <c r="F31" s="3" cm="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F31" s="2" cm="1">
         <f t="array" ref="F31">IF(D31&gt;0,INDEX($M$5:$S$20,D31,E31),0)</f>
         <v>1</v>
       </c>
       <c r="G31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="H31">
-        <f>$B$14-1</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="I31" cm="1">
         <f t="array" ref="I31">IF(G31&gt;0,INDEX($M$5:$S$20,G31,H31),0)</f>
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="J31">
-        <f t="shared" si="2"/>
-        <v>109</v>
+        <f t="shared" si="7"/>
+        <v>1000</v>
+      </c>
+      <c r="N31">
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -1913,59 +1959,93 @@
         <v>16</v>
       </c>
       <c r="B32">
-        <f>$B$14</f>
-        <v>6</v>
-      </c>
-      <c r="C32" s="3" cm="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C32" s="2" cm="1">
         <f t="array" ref="C32">IF(A32&gt;0,INDEX($M$5:$S$20,A32,B32),0)</f>
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="D32">
-        <f>$A$14-A32</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E32">
-        <f>$B$14-1</f>
-        <v>5</v>
-      </c>
-      <c r="F32" s="3" cm="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F32" s="2" cm="1">
         <f t="array" ref="F32">IF(D32&gt;0,INDEX($M$5:$S$20,D32,E32),0)</f>
         <v>0</v>
       </c>
       <c r="G32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="H32">
-        <f>$B$14-1</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="I32" cm="1">
         <f t="array" ref="I32">IF(G32&gt;0,INDEX($M$5:$S$20,G32,H32),0)</f>
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="J32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1000</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="N32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="N37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>16</v>
       </c>
       <c r="B38">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="N38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>SUM(A41:A51)</f>
         <v>16</v>
@@ -1974,26 +2054,32 @@
         <f>SUM(D42:E47)</f>
         <v>51</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
         <v>20</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>21</v>
       </c>
-      <c r="C41" t="s">
-        <v>22</v>
-      </c>
       <c r="D41" t="s">
         <v>0</v>
       </c>
       <c r="E41" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="20">
+      <c r="N41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="17">
         <v>5</v>
       </c>
       <c r="B42">
@@ -2002,17 +2088,17 @@
       <c r="C42">
         <v>5</v>
       </c>
-      <c r="D42" s="3" cm="1">
+      <c r="D42" s="2" cm="1">
         <f t="array" ref="D42">IF(AND(B42&gt;0,A42&gt;0),INDEX($M$5:$S$20,A42,B42),0)</f>
         <v>9</v>
       </c>
-      <c r="E42" s="3" cm="1">
+      <c r="E42" s="2" cm="1">
         <f t="array" ref="E42">IF(AND(C42&gt;0,A42&gt;0),INDEX($M$5:$S$20,A42,C42),0)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="20">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="17">
         <v>4</v>
       </c>
       <c r="B43">
@@ -2021,17 +2107,17 @@
       <c r="C43">
         <v>4</v>
       </c>
-      <c r="D43" s="3" cm="1">
+      <c r="D43" s="2" cm="1">
         <f t="array" ref="D43">IF(AND(B43&gt;0,A43&gt;0),INDEX($M$5:$S$20,A43,B43),0)</f>
         <v>7</v>
       </c>
-      <c r="E43" s="3" cm="1">
+      <c r="E43" s="2" cm="1">
         <f t="array" ref="E43">IF(AND(C43&gt;0,A43&gt;0),INDEX($M$5:$S$20,A43,C43),0)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="20">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="17">
         <v>3</v>
       </c>
       <c r="B44">
@@ -2040,17 +2126,17 @@
       <c r="C44">
         <v>3</v>
       </c>
-      <c r="D44" s="3" cm="1">
+      <c r="D44" s="2" cm="1">
         <f t="array" ref="D44">IF(AND(B44&gt;0,A44&gt;0),INDEX($M$5:$S$20,A44,B44),0)</f>
         <v>5</v>
       </c>
-      <c r="E44" s="3" cm="1">
+      <c r="E44" s="2" cm="1">
         <f t="array" ref="E44">IF(AND(C44&gt;0,A44&gt;0),INDEX($M$5:$S$20,A44,C44),0)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="20">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="17">
         <v>2</v>
       </c>
       <c r="B45">
@@ -2059,17 +2145,17 @@
       <c r="C45">
         <v>2</v>
       </c>
-      <c r="D45" s="3" cm="1">
+      <c r="D45" s="2" cm="1">
         <f t="array" ref="D45">IF(AND(B45&gt;0,A45&gt;0),INDEX($M$5:$S$20,A45,B45),0)</f>
         <v>3</v>
       </c>
-      <c r="E45" s="3" cm="1">
+      <c r="E45" s="2" cm="1">
         <f t="array" ref="E45">IF(AND(C45&gt;0,A45&gt;0),INDEX($M$5:$S$20,A45,C45),0)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="20">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="17">
         <v>1</v>
       </c>
       <c r="B46">
@@ -2078,17 +2164,17 @@
       <c r="C46">
         <v>1</v>
       </c>
-      <c r="D46" s="3" cm="1">
+      <c r="D46" s="2" cm="1">
         <f t="array" ref="D46">IF(AND(B46&gt;0,A46&gt;0),INDEX($M$5:$S$20,A46,B46),0)</f>
         <v>1</v>
       </c>
-      <c r="E46" s="3" cm="1">
+      <c r="E46" s="2" cm="1">
         <f t="array" ref="E46">IF(AND(C46&gt;0,A46&gt;0),INDEX($M$5:$S$20,A46,C46),0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="20">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="17">
         <v>1</v>
       </c>
       <c r="B47">
@@ -2097,11 +2183,11 @@
       <c r="C47">
         <v>0</v>
       </c>
-      <c r="D47" s="3" cm="1">
+      <c r="D47" s="2" cm="1">
         <f t="array" ref="D47">IF(AND(B47&gt;0,A47&gt;0),INDEX($M$5:$S$20,A47,B47),0)</f>
         <v>1</v>
       </c>
-      <c r="E47" s="3" cm="1">
+      <c r="E47" s="2" cm="1">
         <f t="array" ref="E47">IF(AND(C47&gt;0,A47&gt;0),INDEX($M$5:$S$20,A47,C47),0)</f>
         <v>0</v>
       </c>

</xml_diff>